<commit_message>
Updated with current information (still needs work)
</commit_message>
<xml_diff>
--- a/Serial/MCU Serial Info.xlsx
+++ b/Serial/MCU Serial Info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Uni\Robotics\MSL\Serial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bens1\Documents\Uni\Robotics\MSL\MSL_github\MSL_Imperial_2023\Serial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8078D54-4D35-4576-AE2B-0052EB6331D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AC6BC3-5B6F-40DA-936D-2E8ABD398BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="12900" windowHeight="10200" xr2:uid="{4B9EE938-D0BB-4786-875D-7EF06ACADB20}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4B9EE938-D0BB-4786-875D-7EF06ACADB20}"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="140">
   <si>
     <t>Opcode</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Arguments</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>Byte 1</t>
   </si>
   <si>
@@ -108,33 +105,15 @@
     <t>Read actual overall velocity</t>
   </si>
   <si>
-    <t>M1W</t>
-  </si>
-  <si>
     <t>M1R</t>
   </si>
   <si>
-    <t>M2W</t>
-  </si>
-  <si>
     <t>M2R</t>
   </si>
   <si>
-    <t>M3W</t>
-  </si>
-  <si>
     <t>M3R</t>
   </si>
   <si>
-    <t>Write motor 1 speed</t>
-  </si>
-  <si>
-    <t>Write motor 2 speed</t>
-  </si>
-  <si>
-    <t>Write motor 3 speed</t>
-  </si>
-  <si>
     <t>Read actual motor 1 speed</t>
   </si>
   <si>
@@ -150,12 +129,6 @@
     <t>Byte 6</t>
   </si>
   <si>
-    <t>Write to the build in LED</t>
-  </si>
-  <si>
-    <t>status = 1 for on, status = 0 for off</t>
-  </si>
-  <si>
     <t>DIR</t>
   </si>
   <si>
@@ -426,9 +399,6 @@
     <t>motor</t>
   </si>
   <si>
-    <t>int motor, string readwrite, string actualtarget, speed float</t>
-  </si>
-  <si>
     <t>Motor write successful</t>
   </si>
   <si>
@@ -451,6 +421,42 @@
   </si>
   <si>
     <t>'!'</t>
+  </si>
+  <si>
+    <t>int motor, string readwrite, string actualtarget, float speed</t>
+  </si>
+  <si>
+    <t>int led_code</t>
+  </si>
+  <si>
+    <t>led_code = 0 green, 1 red, 2 blue</t>
+  </si>
+  <si>
+    <t>status = 0 off, 1 on, 2 toggle</t>
+  </si>
+  <si>
+    <t>Write to an LED</t>
+  </si>
+  <si>
+    <t>LEDW</t>
+  </si>
+  <si>
+    <t>M1TW</t>
+  </si>
+  <si>
+    <t>M2TW</t>
+  </si>
+  <si>
+    <t>Write motor 2 target speed</t>
+  </si>
+  <si>
+    <t>Write motor 1 target speed</t>
+  </si>
+  <si>
+    <t>Write motor 3 target speed</t>
+  </si>
+  <si>
+    <t>M3TW</t>
   </si>
 </sst>
 </file>
@@ -528,29 +534,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -880,7 +897,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -888,545 +905,575 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62141083-4FF8-47BC-8027-F1F7187F0C70}">
-  <dimension ref="B1:V33"/>
+  <dimension ref="B1:V34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="12" width="9.140625" style="4"/>
+    <col min="13" max="13" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="4"/>
+    <col min="16" max="16" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="53.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="M2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" s="7"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="R3" s="7"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="R4" s="7"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="R6" s="7"/>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B7" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="R7" s="7"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="R8" s="7"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="R10" s="7"/>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="N11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="R11" s="7"/>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="R12" s="7"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="N13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="R13" s="7"/>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="M15" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q15" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="R1" s="4" t="s">
+      <c r="S15" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="Q16" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N21" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="P21" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="R21" s="13">
+        <v>2</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="T21" s="7"/>
+      <c r="U21" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="V21" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N22" s="12"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T22" s="7"/>
+      <c r="U22" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="V22" s="13"/>
+    </row>
+    <row r="23" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="M2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="O23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="P2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>102</v>
-      </c>
-      <c r="R2" s="8"/>
-      <c r="V2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>101</v>
-      </c>
-      <c r="R3" s="8"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>100</v>
-      </c>
-      <c r="R4" s="8"/>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>99</v>
-      </c>
-      <c r="R5" s="8"/>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="P23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R23" s="4">
+        <v>5</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T23" s="7"/>
+    </row>
+    <row r="24" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N24" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P24" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>98</v>
-      </c>
-      <c r="R6" s="8"/>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="R24" s="4">
+        <v>5</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T24" s="7"/>
+    </row>
+    <row r="25" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="P25" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="R25" s="4">
         <v>5</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="S25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P7" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>104</v>
-      </c>
-      <c r="R7" s="8"/>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P8" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>106</v>
-      </c>
-      <c r="R8" s="8"/>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>87</v>
-      </c>
-      <c r="N9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>108</v>
-      </c>
-      <c r="R9" s="8"/>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>109</v>
-      </c>
-      <c r="R10" s="8"/>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>112</v>
-      </c>
-      <c r="R11" s="8"/>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P12" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>114</v>
-      </c>
-      <c r="R12" s="8"/>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="N13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P13" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>116</v>
-      </c>
-      <c r="R13" s="8"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="M15" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>127</v>
-      </c>
-      <c r="S15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="Q16" t="s">
-        <v>128</v>
-      </c>
-      <c r="S16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="21" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O21" t="s">
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="P26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="R26" s="4">
+        <v>5</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="T26" s="7"/>
+    </row>
+    <row r="27" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="R27" s="4">
+        <v>5</v>
+      </c>
+      <c r="S27" s="7"/>
+      <c r="T27" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" s="4">
+        <v>5</v>
+      </c>
+      <c r="S28" s="7"/>
+      <c r="T28" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="R29" s="4">
+        <v>5</v>
+      </c>
+      <c r="S29" s="7"/>
+      <c r="T29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N30" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R30" s="4">
+        <v>5</v>
+      </c>
+      <c r="S30" s="7"/>
+      <c r="T30" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="R31" s="4">
         <v>3</v>
       </c>
-      <c r="P21" t="s">
+      <c r="S31" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T31" s="7"/>
+      <c r="U31" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="14:22" x14ac:dyDescent="0.25">
+      <c r="N32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R32" s="4">
+        <v>3</v>
+      </c>
+      <c r="S32" s="7"/>
+      <c r="T32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="U32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21" t="s">
-        <v>45</v>
-      </c>
-      <c r="T21" s="8"/>
-      <c r="U21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N22" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O22" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" t="s">
-        <v>21</v>
-      </c>
-      <c r="R22">
-        <v>5</v>
-      </c>
-      <c r="S22" t="s">
+    </row>
+    <row r="33" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N33" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R33" s="4">
+        <v>3</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T33" s="7"/>
+      <c r="U33" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="14:21" x14ac:dyDescent="0.25">
+      <c r="N34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R34" s="4">
+        <v>3</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T34" s="7"/>
+      <c r="U34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="T22" s="8"/>
-    </row>
-    <row r="23" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O23" t="s">
-        <v>23</v>
-      </c>
-      <c r="P23" t="s">
-        <v>29</v>
-      </c>
-      <c r="R23">
-        <v>5</v>
-      </c>
-      <c r="S23" t="s">
-        <v>44</v>
-      </c>
-      <c r="T23" s="8"/>
-    </row>
-    <row r="24" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" t="s">
-        <v>25</v>
-      </c>
-      <c r="P24" t="s">
-        <v>30</v>
-      </c>
-      <c r="R24">
-        <v>5</v>
-      </c>
-      <c r="S24" t="s">
-        <v>44</v>
-      </c>
-      <c r="T24" s="8"/>
-    </row>
-    <row r="25" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N25" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O25" t="s">
-        <v>27</v>
-      </c>
-      <c r="P25" t="s">
-        <v>31</v>
-      </c>
-      <c r="R25">
-        <v>5</v>
-      </c>
-      <c r="S25" t="s">
-        <v>44</v>
-      </c>
-      <c r="T25" s="8"/>
-    </row>
-    <row r="26" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N26" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O26" t="s">
-        <v>20</v>
-      </c>
-      <c r="P26" t="s">
-        <v>22</v>
-      </c>
-      <c r="R26">
-        <v>5</v>
-      </c>
-      <c r="S26" s="8"/>
-      <c r="T26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N27" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O27" t="s">
-        <v>24</v>
-      </c>
-      <c r="P27" t="s">
-        <v>32</v>
-      </c>
-      <c r="R27">
-        <v>5</v>
-      </c>
-      <c r="S27" s="8"/>
-      <c r="T27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N28" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O28" t="s">
-        <v>26</v>
-      </c>
-      <c r="P28" t="s">
-        <v>33</v>
-      </c>
-      <c r="R28">
-        <v>5</v>
-      </c>
-      <c r="S28" s="8"/>
-      <c r="T28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O29" t="s">
-        <v>28</v>
-      </c>
-      <c r="P29" t="s">
-        <v>34</v>
-      </c>
-      <c r="R29">
-        <v>5</v>
-      </c>
-      <c r="S29" s="8"/>
-      <c r="T29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O30" t="s">
-        <v>40</v>
-      </c>
-      <c r="P30" t="s">
-        <v>41</v>
-      </c>
-      <c r="R30">
-        <v>3</v>
-      </c>
-      <c r="S30" t="s">
-        <v>47</v>
-      </c>
-      <c r="T30" s="8"/>
-      <c r="U30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O31" t="s">
-        <v>39</v>
-      </c>
-      <c r="P31" t="s">
-        <v>42</v>
-      </c>
-      <c r="R31">
-        <v>3</v>
-      </c>
-      <c r="S31" s="8"/>
-      <c r="T31" t="s">
-        <v>47</v>
-      </c>
-      <c r="U31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O32" t="s">
-        <v>49</v>
-      </c>
-      <c r="P32" t="s">
-        <v>50</v>
-      </c>
-      <c r="R32">
-        <v>3</v>
-      </c>
-      <c r="S32" t="s">
-        <v>51</v>
-      </c>
-      <c r="T32" s="8"/>
-      <c r="U32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N33" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="O33" t="s">
-        <v>48</v>
-      </c>
-      <c r="P33" t="s">
-        <v>50</v>
-      </c>
-      <c r="R33">
-        <v>3</v>
-      </c>
-      <c r="S33" t="s">
-        <v>51</v>
-      </c>
-      <c r="T33" s="8"/>
-      <c r="U33" t="s">
-        <v>53</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="R21:R22"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="V21:V22"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="N1:N1048576">
+  <conditionalFormatting sqref="N1:N21 N23:N1048576">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"n"</formula>
     </cfRule>
@@ -1434,7 +1481,7 @@
       <formula>"y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N1:N1048576">
+  <conditionalFormatting sqref="N1:N21 N23:N1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"wip"</formula>
     </cfRule>
@@ -1461,32 +1508,32 @@
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>1</v>
@@ -1497,7 +1544,7 @@
         <v>101</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1505,7 +1552,7 @@
         <v>102</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1513,7 +1560,7 @@
         <v>103</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1521,7 +1568,7 @@
         <v>105</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1529,7 +1576,7 @@
         <v>106</v>
       </c>
       <c r="E14" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1537,7 +1584,7 @@
         <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1545,7 +1592,7 @@
         <v>111</v>
       </c>
       <c r="E16" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
@@ -1553,7 +1600,7 @@
         <v>125</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
@@ -1561,7 +1608,7 @@
         <v>120</v>
       </c>
       <c r="E18" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
@@ -1569,7 +1616,7 @@
         <v>130</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
@@ -1577,7 +1624,7 @@
         <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
@@ -1585,7 +1632,7 @@
         <v>200</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
@@ -1593,7 +1640,7 @@
         <v>202</v>
       </c>
       <c r="E22" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
@@ -1601,7 +1648,7 @@
         <v>203</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
@@ -1609,7 +1656,7 @@
         <v>205</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
@@ -1617,7 +1664,7 @@
         <v>206</v>
       </c>
       <c r="E25" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
@@ -1625,7 +1672,7 @@
         <v>210</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
@@ -1633,7 +1680,7 @@
         <v>211</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.25">
@@ -1641,7 +1688,7 @@
         <v>220</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
@@ -1649,7 +1696,7 @@
         <v>225</v>
       </c>
       <c r="E29" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.25">
@@ -1657,7 +1704,7 @@
         <v>230</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
@@ -1665,7 +1712,7 @@
         <v>241</v>
       </c>
       <c r="E31" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.25">
@@ -1673,7 +1720,7 @@
         <v>245</v>
       </c>
       <c r="E32" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
@@ -1681,7 +1728,7 @@
         <v>400</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
@@ -1689,7 +1736,7 @@
         <v>401</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
@@ -1697,7 +1744,7 @@
         <v>402</v>
       </c>
       <c r="E35" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
@@ -1705,7 +1752,7 @@
         <v>403</v>
       </c>
       <c r="E36" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
@@ -1713,7 +1760,7 @@
         <v>404</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
@@ -1721,7 +1768,7 @@
         <v>405</v>
       </c>
       <c r="E38" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
@@ -1729,7 +1776,7 @@
         <v>406</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.25">
@@ -1737,7 +1784,7 @@
         <v>410</v>
       </c>
       <c r="E40" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.25">
@@ -1745,7 +1792,7 @@
         <v>411</v>
       </c>
       <c r="E41" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.25">
@@ -1753,7 +1800,7 @@
         <v>412</v>
       </c>
       <c r="E42" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.25">
@@ -1761,7 +1808,7 @@
         <v>420</v>
       </c>
       <c r="E43" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.25">
@@ -1769,7 +1816,7 @@
         <v>425</v>
       </c>
       <c r="E44" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="4:5" x14ac:dyDescent="0.25">
@@ -1777,7 +1824,7 @@
         <v>430</v>
       </c>
       <c r="E45" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="4:5" x14ac:dyDescent="0.25">
@@ -1785,7 +1832,7 @@
         <v>440</v>
       </c>
       <c r="E46" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="4:5" x14ac:dyDescent="0.25">
@@ -1793,7 +1840,7 @@
         <v>441</v>
       </c>
       <c r="E47" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="4:5" x14ac:dyDescent="0.25">
@@ -1801,7 +1848,7 @@
         <v>445</v>
       </c>
       <c r="E48" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>